<commit_message>
Updated the Unit test cases
Added few test cases based on the new changes.
</commit_message>
<xml_diff>
--- a/Unit Test Cases.xlsx
+++ b/Unit Test Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>TEST CASE ID</t>
   </si>
@@ -83,13 +83,45 @@
     <t>User should able to remove 
 the items from the multi 
 select field</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>Get all selected values button should fetch and 
+display the items</t>
+  </si>
+  <si>
+    <t>User should able to get all the
+selected items.
+If no values selected, User
+should populated with
+respective message</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>Selecting the options in the dropdown should display it
+as selected by marking with √ mark.
+User can remove the selected option by re-selecting
+the same selected option. √ mark should be removed
+along with items in the multiselect field removed.</t>
+  </si>
+  <si>
+    <t>Selected Option should be provided with
+tick √ mark to the user.
+Re-selcting the option should
+remove the √ mark and remove 
+the items in multiselect field as
+well</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -112,8 +144,14 @@
       <color rgb="FF20A603"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +162,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD4D4D4"/>
         <bgColor rgb="FFD4D4D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -147,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -162,6 +206,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,6 +549,60 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" ht="95.25" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f>HYPERLINK("https://gsprasanna.github.io/Multi-Select-Dropdown-Component/","1) Go to site : https://gsprasanna.github.io/Multi-Select-Dropdown-Component/
+2) Click ""Get all selected valued"" Button.
+3) Alert should show all the selected values. 
+    If no values selected, show the ""Please select items"" message to user.")</f>
+        <v>1) Go to site : https://gsprasanna.github.io/Multi-Select-Dropdown-Component/
+2) Click "Get all selected valued" Button.
+3) Alert should show all the selected values. 
+    If no values selected, show the "Please select items" message to user.</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="95.25" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f>HYPERLINK("https://gsprasanna.github.io/Multi-Select-Dropdown-Component/","1) Go to site : https://gsprasanna.github.io/Multi-Select-Dropdown-Component/
+2) Select the options in the dropdown.
+3) Selected option should added to multiselect field and marked with √ mark.
+4) Re-selecting the selected option.")</f>
+        <v>1) Go to site : https://gsprasanna.github.io/Multi-Select-Dropdown-Component/
+2) Select the options in the dropdown.
+3) Selected option should added to multiselect field and marked with √ mark.
+4) Re-selecting the selected option.</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>